<commit_message>
Change ILED to 0
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_PWR_CCS_GAS_START_2027.xlsx
+++ b/SuppXLS/Scen_B_PWR_CCS_GAS_START_2027.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Ireland-model\main\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4CE801-BF64-4BE9-BA40-94FE3AD2B903}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9F4025-E71F-4400-981F-5443379CFF2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13110" yWindow="6525" windowWidth="28110" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UPD" sheetId="11" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>NCAP_START</t>
+  </si>
+  <si>
+    <t>NCAP_ILED</t>
   </si>
 </sst>
 </file>
@@ -1235,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1389,6 +1392,82 @@
         <v>21</v>
       </c>
     </row>
+    <row r="8" spans="1:16">
+      <c r="D8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="D9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="D10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="D11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>